<commit_message>
se modifican Endosos Adicional Devolucion ABM Conductor y se agregan MenuLateral_Vehiculo.rxrec y MenuLateral_ComisionesDesc
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Endoso - ABM_Accesorios.xlsx
+++ b/Sura/DataSource - Endoso - ABM_Accesorios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36087A46-3B1E-4644-B434-9FE43126F49C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9451F22-F8A7-4DB4-949F-E19E2C45FF8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
     <t>su</t>
   </si>
   <si>
-    <t>04104016463</t>
+    <t>04104016436</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>